<commit_message>
Updated detailed indicator quantile results.
</commit_message>
<xml_diff>
--- a/output/ScriptResults/Database_Thresholds_details.xlsx
+++ b/output/ScriptResults/Database_Thresholds_details.xlsx
@@ -149,7 +149,7 @@
     <t xml:space="preserve">All_CORAL_Parameters-2023-Dec-13.txt</t>
   </si>
   <si>
-    <t xml:space="preserve">IndicatorQuantiles.R, Git Commit ID: 54e4488a188edf59eafc4b9cfe53dc7125db7b32</t>
+    <t xml:space="preserve">IndicatorQuantiles.R, Git Commit ID: 0e4152332be22faf035a2e2fc83ad2cca4c8a7fc</t>
   </si>
   <si>
     <t xml:space="preserve">Percent Cover</t>
@@ -1356,7 +1356,7 @@
         <v>178</v>
       </c>
       <c r="AH2" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI2" t="s">
         <v>44</v>
@@ -1467,7 +1467,7 @@
         <v>2001</v>
       </c>
       <c r="AH3" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI3" t="s">
         <v>44</v>
@@ -1578,7 +1578,7 @@
         <v>6553</v>
       </c>
       <c r="AH4" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI4" t="s">
         <v>44</v>
@@ -1689,7 +1689,7 @@
         <v>175</v>
       </c>
       <c r="AH5" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI5" t="s">
         <v>44</v>
@@ -1800,7 +1800,7 @@
         <v>4456</v>
       </c>
       <c r="AH6" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI6" t="s">
         <v>44</v>
@@ -1911,7 +1911,7 @@
         <v>3667</v>
       </c>
       <c r="AH7" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI7" t="s">
         <v>44</v>
@@ -2022,7 +2022,7 @@
         <v>27370</v>
       </c>
       <c r="AH8" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI8" t="s">
         <v>68</v>
@@ -2133,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI9" t="s">
         <v>44</v>
@@ -2244,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="AH10" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI10" t="s">
         <v>68</v>
@@ -2355,7 +2355,7 @@
         <v>27370</v>
       </c>
       <c r="AH11" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI11" t="s">
         <v>85</v>
@@ -2466,7 +2466,7 @@
         <v>16</v>
       </c>
       <c r="AH12" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI12" t="s">
         <v>90</v>
@@ -2577,7 +2577,7 @@
         <v>3667</v>
       </c>
       <c r="AH13" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI13" t="s">
         <v>99</v>
@@ -2688,7 +2688,7 @@
         <v>3667</v>
       </c>
       <c r="AH14" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI14" t="s">
         <v>99</v>
@@ -2799,7 +2799,7 @@
         <v>0</v>
       </c>
       <c r="AH15" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI15" t="s">
         <v>99</v>
@@ -2910,7 +2910,7 @@
         <v>0</v>
       </c>
       <c r="AH16" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI16" t="s">
         <v>99</v>
@@ -3021,7 +3021,7 @@
         <v>34085</v>
       </c>
       <c r="AH17" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI17" t="s">
         <v>113</v>
@@ -3132,7 +3132,7 @@
         <v>34085</v>
       </c>
       <c r="AH18" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI18" t="s">
         <v>113</v>
@@ -3243,7 +3243,7 @@
         <v>98</v>
       </c>
       <c r="AH19" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI19" t="s">
         <v>121</v>
@@ -3354,7 +3354,7 @@
         <v>0</v>
       </c>
       <c r="AH20" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI20" t="s">
         <v>121</v>
@@ -3465,7 +3465,7 @@
         <v>17</v>
       </c>
       <c r="AH21" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI21" t="s">
         <v>121</v>
@@ -3576,7 +3576,7 @@
         <v>24</v>
       </c>
       <c r="AH22" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI22" t="s">
         <v>121</v>
@@ -3689,7 +3689,7 @@
         <v>24</v>
       </c>
       <c r="AH23" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI23" t="s">
         <v>121</v>
@@ -3802,7 +3802,7 @@
         <v>24</v>
       </c>
       <c r="AH24" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI24" t="s">
         <v>121</v>
@@ -3915,7 +3915,7 @@
         <v>24</v>
       </c>
       <c r="AH25" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI25" t="s">
         <v>121</v>
@@ -4028,7 +4028,7 @@
         <v>24</v>
       </c>
       <c r="AH26" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI26" t="s">
         <v>121</v>
@@ -4139,7 +4139,7 @@
         <v>73</v>
       </c>
       <c r="AH27" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI27" t="s">
         <v>121</v>
@@ -4252,7 +4252,7 @@
         <v>73</v>
       </c>
       <c r="AH28" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI28" t="s">
         <v>121</v>
@@ -4365,7 +4365,7 @@
         <v>73</v>
       </c>
       <c r="AH29" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI29" t="s">
         <v>121</v>
@@ -4478,7 +4478,7 @@
         <v>73</v>
       </c>
       <c r="AH30" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI30" t="s">
         <v>121</v>
@@ -4591,7 +4591,7 @@
         <v>73</v>
       </c>
       <c r="AH31" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI31" t="s">
         <v>121</v>
@@ -4702,7 +4702,7 @@
         <v>71</v>
       </c>
       <c r="AH32" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI32" t="s">
         <v>121</v>
@@ -4815,7 +4815,7 @@
         <v>71</v>
       </c>
       <c r="AH33" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI33" t="s">
         <v>121</v>
@@ -4928,7 +4928,7 @@
         <v>71</v>
       </c>
       <c r="AH34" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI34" t="s">
         <v>121</v>
@@ -5041,7 +5041,7 @@
         <v>71</v>
       </c>
       <c r="AH35" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI35" t="s">
         <v>121</v>
@@ -5154,7 +5154,7 @@
         <v>71</v>
       </c>
       <c r="AH36" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI36" t="s">
         <v>121</v>
@@ -5265,7 +5265,7 @@
         <v>1281</v>
       </c>
       <c r="AH37" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI37" t="s">
         <v>121</v>
@@ -5378,7 +5378,7 @@
         <v>1281</v>
       </c>
       <c r="AH38" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI38" t="s">
         <v>121</v>
@@ -5491,7 +5491,7 @@
         <v>1281</v>
       </c>
       <c r="AH39" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI39" t="s">
         <v>121</v>
@@ -5604,7 +5604,7 @@
         <v>1281</v>
       </c>
       <c r="AH40" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI40" t="s">
         <v>121</v>
@@ -5717,7 +5717,7 @@
         <v>1281</v>
       </c>
       <c r="AH41" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI41" t="s">
         <v>121</v>
@@ -5830,7 +5830,7 @@
         <v>1281</v>
       </c>
       <c r="AH42" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI42" t="s">
         <v>121</v>
@@ -5941,7 +5941,7 @@
         <v>17703</v>
       </c>
       <c r="AH43" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI43" t="s">
         <v>159</v>
@@ -6052,7 +6052,7 @@
         <v>0</v>
       </c>
       <c r="AH44" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI44" t="s">
         <v>159</v>
@@ -6163,7 +6163,7 @@
         <v>27370</v>
       </c>
       <c r="AH45" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI45" t="s">
         <v>168</v>
@@ -6274,7 +6274,7 @@
         <v>27370</v>
       </c>
       <c r="AH46" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI46" t="s">
         <v>159</v>
@@ -6385,7 +6385,7 @@
         <v>34168</v>
       </c>
       <c r="AH47" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI47" t="s">
         <v>159</v>
@@ -6496,7 +6496,7 @@
         <v>34168</v>
       </c>
       <c r="AH48" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI48" t="s">
         <v>159</v>
@@ -6607,7 +6607,7 @@
         <v>0</v>
       </c>
       <c r="AH49" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI49" t="s">
         <v>68</v>
@@ -6718,7 +6718,7 @@
         <v>2438</v>
       </c>
       <c r="AH50" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI50" t="s">
         <v>159</v>
@@ -6829,7 +6829,7 @@
         <v>10</v>
       </c>
       <c r="AH51" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI51" t="s">
         <v>179</v>
@@ -6940,7 +6940,7 @@
         <v>604</v>
       </c>
       <c r="AH52" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI52" t="s">
         <v>183</v>
@@ -7051,7 +7051,7 @@
         <v>1</v>
       </c>
       <c r="AH53" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI53" t="s">
         <v>186</v>
@@ -7162,7 +7162,7 @@
         <v>346</v>
       </c>
       <c r="AH54" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI54" t="s">
         <v>189</v>
@@ -7273,7 +7273,7 @@
         <v>27</v>
       </c>
       <c r="AH55" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI55" t="s">
         <v>194</v>
@@ -7384,7 +7384,7 @@
         <v>3</v>
       </c>
       <c r="AH56" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI56" t="s">
         <v>197</v>
@@ -7495,7 +7495,7 @@
         <v>210</v>
       </c>
       <c r="AH57" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI57" t="s">
         <v>199</v>
@@ -7606,7 +7606,7 @@
         <v>40</v>
       </c>
       <c r="AH58" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI58" t="s">
         <v>201</v>
@@ -7717,7 +7717,7 @@
         <v>126</v>
       </c>
       <c r="AH59" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI59" t="s">
         <v>203</v>
@@ -7828,7 +7828,7 @@
         <v>317</v>
       </c>
       <c r="AH60" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI60" t="s">
         <v>206</v>
@@ -7939,7 +7939,7 @@
         <v>95</v>
       </c>
       <c r="AH61" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI61" t="s">
         <v>209</v>
@@ -8050,7 +8050,7 @@
         <v>38</v>
       </c>
       <c r="AH62" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI62" t="s">
         <v>213</v>
@@ -8161,7 +8161,7 @@
         <v>4</v>
       </c>
       <c r="AH63" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI63" t="s">
         <v>216</v>
@@ -8272,7 +8272,7 @@
         <v>102</v>
       </c>
       <c r="AH64" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI64" t="s">
         <v>219</v>
@@ -8383,7 +8383,7 @@
         <v>5</v>
       </c>
       <c r="AH65" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI65" t="s">
         <v>221</v>
@@ -8494,7 +8494,7 @@
         <v>2606</v>
       </c>
       <c r="AH66" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI66" t="s">
         <v>223</v>
@@ -8605,7 +8605,7 @@
         <v>30</v>
       </c>
       <c r="AH67" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI67" t="s">
         <v>225</v>
@@ -8716,7 +8716,7 @@
         <v>33</v>
       </c>
       <c r="AH68" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI68" t="s">
         <v>227</v>
@@ -8827,7 +8827,7 @@
         <v>8</v>
       </c>
       <c r="AH69" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI69" t="s">
         <v>230</v>
@@ -8938,7 +8938,7 @@
         <v>8</v>
       </c>
       <c r="AH70" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI70" t="s">
         <v>230</v>
@@ -9049,7 +9049,7 @@
         <v>3</v>
       </c>
       <c r="AH71" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI71" t="s">
         <v>233</v>
@@ -9160,7 +9160,7 @@
         <v>20</v>
       </c>
       <c r="AH72" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI72" t="s">
         <v>236</v>
@@ -9271,7 +9271,7 @@
         <v>2061</v>
       </c>
       <c r="AH73" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI73" t="s">
         <v>238</v>
@@ -9382,7 +9382,7 @@
         <v>2</v>
       </c>
       <c r="AH74" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI74" t="s">
         <v>241</v>
@@ -9493,7 +9493,7 @@
         <v>42765</v>
       </c>
       <c r="AH75" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI75" t="s">
         <v>243</v>
@@ -9604,7 +9604,7 @@
         <v>48795</v>
       </c>
       <c r="AH76" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI76" t="s">
         <v>244</v>
@@ -9715,7 +9715,7 @@
         <v>12171</v>
       </c>
       <c r="AH77" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI77" t="s">
         <v>245</v>
@@ -9826,7 +9826,7 @@
         <v>3602</v>
       </c>
       <c r="AH78" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI78" t="s">
         <v>246</v>
@@ -9937,7 +9937,7 @@
         <v>59242</v>
       </c>
       <c r="AH79" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI79" t="s">
         <v>247</v>
@@ -10048,7 +10048,7 @@
         <v>617164</v>
       </c>
       <c r="AH80" t="n">
-        <v>30656</v>
+        <v>25596</v>
       </c>
       <c r="AI80" t="s">
         <v>248</v>

</xml_diff>